<commit_message>
Week 4 - CRUD UI tests + DDT + CI
</commit_message>
<xml_diff>
--- a/docs/test_cases_ui.xlsx
+++ b/docs/test_cases_ui.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LTH\nam_4\PythonProject\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D502DE19-86DB-4766-BEA3-7E415A03CF23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A443C1-ED9A-4482-9F82-382F96EE238E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="3" activeTab="4" xr2:uid="{E972E92D-3E80-4BBC-AE0A-51564C9880A0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{E972E92D-3E80-4BBC-AE0A-51564C9880A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="153">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -75,15 +75,9 @@
     <t>TC_UI_LOGIN_06</t>
   </si>
   <si>
-    <t>TC_UI_LOGIN_07</t>
-  </si>
-  <si>
     <t>User hợp lệ</t>
   </si>
   <si>
-    <t>User bị disable</t>
-  </si>
-  <si>
     <t>Username trống</t>
   </si>
   <si>
@@ -103,9 +97,6 @@
   </si>
   <si>
     <t>Kiểm tra login sai password</t>
-  </si>
-  <si>
-    <t>Login với tài khoản bị khóa</t>
   </si>
   <si>
     <t>Kiểm tra phân biệt chữ hoa/thường</t>
@@ -162,10 +153,6 @@
 3. Click Login</t>
   </si>
   <si>
-    <t>1. Nhập user disable 
-2. Click Login</t>
-  </si>
-  <si>
     <t>1. Nhập Username = “Admin” 
 2. Nhập đúng password</t>
   </si>
@@ -177,9 +164,6 @@
     <t>Username="Admin"</t>
   </si>
   <si>
-    <t>username=lockedUser</t>
-  </si>
-  <si>
     <t>password=""</t>
   </si>
   <si>
@@ -187,12 +171,6 @@
   </si>
   <si>
     <t>Hiển thị “Required”</t>
-  </si>
-  <si>
-    <t>Hiển thị “Account disabled”</t>
-  </si>
-  <si>
-    <t>Hiển thị Invalid (case-sensitive)</t>
   </si>
   <si>
     <t>Quay về màn hình Login</t>
@@ -607,7 +585,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -615,21 +593,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -969,29 +939,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D08F8658-DF27-4161-BFC6-50B1F0DB53CC}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>16</v>
+      <c r="B1" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -1003,189 +972,159 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="5" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="9" t="s">
+      <c r="D6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="5" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="8" t="s">
+    </row>
+    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="9" t="s">
+      <c r="D7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="5" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-    </row>
-    <row r="10" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1210,7 +1149,7 @@
     <col min="6" max="6" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1224,170 +1163,170 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:6" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B9" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="C9" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="F2" s="7" t="s">
+      <c r="E9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1414,7 +1353,7 @@
     <col min="6" max="6" width="25.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1428,170 +1367,170 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:6" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B9" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="C9" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="E8" s="7" t="s">
+      <c r="E9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>124</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1616,7 +1555,7 @@
     <col min="4" max="4" width="22.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1631,59 +1570,59 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C5" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D5" s="4" t="s">
         <v>140</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -1696,7 +1635,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ABEE569-A1CB-4195-AD95-A50AB2A4447D}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -1708,7 +1647,7 @@
     <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1722,46 +1661,46 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="D3" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+    </row>
+    <row r="4" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="D4" s="4" t="s">
         <v>152</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>